<commit_message>
Fixed parameters and updated notes and datasets for various fields.
</commit_message>
<xml_diff>
--- a/10550_0020.xlsx
+++ b/10550_0020.xlsx
@@ -5867,131 +5867,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId230"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>599</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="231" name="Image 231" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId231"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>599</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="232" name="Image 232" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId232"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>599</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="233" name="Image 233" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId233"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>13</col>
-      <colOff>0</colOff>
-      <row>599</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="234" name="Image 234" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId234"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>17</col>
-      <colOff>0</colOff>
-      <row>599</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="235" name="Image 235" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId235"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6294,7 +6169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7083,14 +6958,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>105.7062490_0.0222487_10550_0020_18</t>
+          <t>105.7364186_0.2367483_10550_0020_18</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>105.706249</v>
+        <v>105.7364186</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0222487</v>
+        <v>0.2367483</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -7099,41 +6974,41 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>cuts/105.7062490,0.0222487_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.7364186,0.2367483_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>cuts/105.7062490,0.0222487_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.7364186,0.2367483_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>cuts/105.7062490,0.0222487_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.7364186,0.2367483_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>cuts/105.7062490,0.0222487_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.7364186,0.2367483_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>cuts/105.7062490,0.0222487_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.7364186,0.2367483_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>105.7364186_0.2367483_10550_0020_19</t>
+          <t>105.7977563_0.4487473_10550_0020_19</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>105.7364186</v>
+        <v>105.7977563</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2367483</v>
+        <v>0.4487473</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -7142,41 +7017,41 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>cuts/105.7364186,0.2367483_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.7977563,0.4487473_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>cuts/105.7364186,0.2367483_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.7977563,0.4487473_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>cuts/105.7364186,0.2367483_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.7977563,0.4487473_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>cuts/105.7364186,0.2367483_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.7977563,0.4487473_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>cuts/105.7364186,0.2367483_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.7977563,0.4487473_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>105.7977563_0.4487473_10550_0020_20</t>
+          <t>105.6057528_0.5339163_10550_0020_20</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>105.7977563</v>
+        <v>105.6057528</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4487473</v>
+        <v>0.5339163</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -7185,41 +7060,41 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>cuts/105.7977563,0.4487473_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.6057528,0.5339163_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>cuts/105.7977563,0.4487473_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.6057528,0.5339163_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>cuts/105.7977563,0.4487473_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.6057528,0.5339163_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>cuts/105.7977563,0.4487473_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.6057528,0.5339163_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>cuts/105.7977563,0.4487473_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.6057528,0.5339163_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>105.6057528_0.5339163_10550_0020_21</t>
+          <t>105.6185861_0.4862496_10550_0020_21</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>105.6057528</v>
+        <v>105.6185861</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5339163</v>
+        <v>0.4862496</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -7228,41 +7103,41 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>cuts/105.6057528,0.5339163_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.6185861,0.4862496_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>cuts/105.6057528,0.5339163_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.6185861,0.4862496_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>cuts/105.6057528,0.5339163_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.6185861,0.4862496_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>cuts/105.6057528,0.5339163_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.6185861,0.4862496_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>cuts/105.6057528,0.5339163_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.6185861,0.4862496_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>105.6185861_0.4862496_10550_0020_22</t>
+          <t>105.8562640_0.7430795_10550_0020_22</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>105.6185861</v>
+        <v>105.856264</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4862496</v>
+        <v>0.7430795</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -7271,41 +7146,41 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>cuts/105.6185861,0.4862496_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.8562640,0.7430795_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>cuts/105.6185861,0.4862496_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.8562640,0.7430795_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>cuts/105.6185861,0.4862496_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.8562640,0.7430795_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>cuts/105.6185861,0.4862496_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.8562640,0.7430795_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>cuts/105.6185861,0.4862496_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.8562640,0.7430795_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>105.8562640_0.7430795_10550_0020_23</t>
+          <t>105.4839160_0.8152500_10550_0020_23</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>105.856264</v>
+        <v>105.483916</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7430795</v>
+        <v>0.81525</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -7314,41 +7189,41 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>cuts/105.8562640,0.7430795_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4839160,0.8152500_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>cuts/105.8562640,0.7430795_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4839160,0.8152500_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>cuts/105.8562640,0.7430795_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4839160,0.8152500_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>cuts/105.8562640,0.7430795_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4839160,0.8152500_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>cuts/105.8562640,0.7430795_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4839160,0.8152500_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>105.4839160_0.8152500_10550_0020_24</t>
+          <t>105.6207551_0.8000829_10550_0020_24</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>105.483916</v>
+        <v>105.6207551</v>
       </c>
       <c r="C25" t="n">
-        <v>0.81525</v>
+        <v>0.8000829</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -7357,41 +7232,41 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>cuts/105.4839160,0.8152500_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.6207551,0.8000829_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>cuts/105.4839160,0.8152500_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.6207551,0.8000829_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>cuts/105.4839160,0.8152500_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.6207551,0.8000829_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>cuts/105.4839160,0.8152500_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.6207551,0.8000829_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>cuts/105.4839160,0.8152500_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.6207551,0.8000829_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>105.6207551_0.8000829_10550_0020_25</t>
+          <t>105.5130838_0.6707500_10550_0020_25</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>105.6207551</v>
+        <v>105.5130838</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8000829</v>
+        <v>0.67075</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -7400,41 +7275,41 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>cuts/105.6207551,0.8000829_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.5130838,0.6707500_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>cuts/105.6207551,0.8000829_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.5130838,0.6707500_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>cuts/105.6207551,0.8000829_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.5130838,0.6707500_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>cuts/105.6207551,0.8000829_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.5130838,0.6707500_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>cuts/105.6207551,0.8000829_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.5130838,0.6707500_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>105.5130838_0.6707500_10550_0020_26</t>
+          <t>105.5319176_0.5567500_10550_0020_26</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>105.5130838</v>
+        <v>105.5319176</v>
       </c>
       <c r="C27" t="n">
-        <v>0.67075</v>
+        <v>0.55675</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -7443,41 +7318,41 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>cuts/105.5130838,0.6707500_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.5319176,0.5567500_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>cuts/105.5130838,0.6707500_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.5319176,0.5567500_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>cuts/105.5130838,0.6707500_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.5319176,0.5567500_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>cuts/105.5130838,0.6707500_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.5319176,0.5567500_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>cuts/105.5130838,0.6707500_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.5319176,0.5567500_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>105.5319176_0.5567500_10550_0020_27</t>
+          <t>105.5240841_0.6047500_10550_0020_27</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>105.5319176</v>
+        <v>105.5240841</v>
       </c>
       <c r="C28" t="n">
-        <v>0.55675</v>
+        <v>0.60475</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -7486,41 +7361,41 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>cuts/105.5319176,0.5567500_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.5240841,0.6047500_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>cuts/105.5319176,0.5567500_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.5240841,0.6047500_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>cuts/105.5319176,0.5567500_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.5240841,0.6047500_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>cuts/105.5319176,0.5567500_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.5240841,0.6047500_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>cuts/105.5319176,0.5567500_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.5240841,0.6047500_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>105.5240841_0.6047500_10550_0020_28</t>
+          <t>105.4732496_0.3519166_10550_0020_28</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>105.5240841</v>
+        <v>105.4732496</v>
       </c>
       <c r="C29" t="n">
-        <v>0.60475</v>
+        <v>0.3519166</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -7529,41 +7404,41 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>cuts/105.5240841,0.6047500_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4732496,0.3519166_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>cuts/105.5240841,0.6047500_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4732496,0.3519166_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>cuts/105.5240841,0.6047500_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4732496,0.3519166_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>cuts/105.5240841,0.6047500_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4732496,0.3519166_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>cuts/105.5240841,0.6047500_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4732496,0.3519166_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>105.4732496_0.3519166_10550_0020_29</t>
+          <t>105.4365838_-0.0332501_10550_0020_29</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>105.4732496</v>
+        <v>105.4365838</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3519166</v>
+        <v>-0.0332501</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -7572,41 +7447,41 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>cuts/105.4732496,0.3519166_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4365838,-0.0332501_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>cuts/105.4732496,0.3519166_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4365838,-0.0332501_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>cuts/105.4732496,0.3519166_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4365838,-0.0332501_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>cuts/105.4732496,0.3519166_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4365838,-0.0332501_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>cuts/105.4732496,0.3519166_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4365838,-0.0332501_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>105.4365838_-0.0332501_10550_0020_30</t>
+          <t>105.3889170_0.0470830_10550_0020_30</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>105.4365838</v>
+        <v>105.388917</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.0332501</v>
+        <v>0.047083</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -7615,41 +7490,41 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>cuts/105.4365838,-0.0332501_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.3889170,0.0470830_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>cuts/105.4365838,-0.0332501_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.3889170,0.0470830_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>cuts/105.4365838,-0.0332501_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.3889170,0.0470830_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>cuts/105.4365838,-0.0332501_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.3889170,0.0470830_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>cuts/105.4365838,-0.0332501_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.3889170,0.0470830_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>105.3889170_0.0470830_10550_0020_31</t>
+          <t>105.4277499_0.1277498_10550_0020_31</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>105.388917</v>
+        <v>105.4277499</v>
       </c>
       <c r="C32" t="n">
-        <v>0.047083</v>
+        <v>0.1277498</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -7658,41 +7533,41 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>cuts/105.3889170,0.0470830_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4277499,0.1277498_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>cuts/105.3889170,0.0470830_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4277499,0.1277498_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>cuts/105.3889170,0.0470830_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4277499,0.1277498_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>cuts/105.3889170,0.0470830_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4277499,0.1277498_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>cuts/105.3889170,0.0470830_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4277499,0.1277498_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>105.4277499_0.1277498_10550_0020_32</t>
+          <t>105.3647485_0.2809161_10550_0020_32</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>105.4277499</v>
+        <v>105.3647485</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1277498</v>
+        <v>0.2809161</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -7701,41 +7576,41 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>cuts/105.4277499,0.1277498_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.3647485,0.2809161_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>cuts/105.4277499,0.1277498_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.3647485,0.2809161_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>cuts/105.4277499,0.1277498_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.3647485,0.2809161_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>cuts/105.4277499,0.1277498_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.3647485,0.2809161_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>cuts/105.4277499,0.1277498_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.3647485,0.2809161_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>105.3647485_0.2809161_10550_0020_33</t>
+          <t>105.2984131_0.3884154_10550_0020_33</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>105.3647485</v>
+        <v>105.2984131</v>
       </c>
       <c r="C34" t="n">
-        <v>0.2809161</v>
+        <v>0.3884154</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -7744,41 +7619,41 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>cuts/105.3647485,0.2809161_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.2984131,0.3884154_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>cuts/105.3647485,0.2809161_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.2984131,0.3884154_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>cuts/105.3647485,0.2809161_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.2984131,0.3884154_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>cuts/105.3647485,0.2809161_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.2984131,0.3884154_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>cuts/105.3647485,0.2809161_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.2984131,0.3884154_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>105.2984131_0.3884154_10550_0020_34</t>
+          <t>105.3749015_0.4830706_10550_0020_34</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>105.2984131</v>
+        <v>105.3749015</v>
       </c>
       <c r="C35" t="n">
-        <v>0.3884154</v>
+        <v>0.4830706</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -7787,41 +7662,41 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>cuts/105.2984131,0.3884154_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.3749015,0.4830706_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>cuts/105.2984131,0.3884154_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.3749015,0.4830706_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>cuts/105.2984131,0.3884154_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.3749015,0.4830706_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>cuts/105.2984131,0.3884154_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.3749015,0.4830706_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>cuts/105.2984131,0.3884154_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.3749015,0.4830706_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>105.3749015_0.4830706_10550_0020_35</t>
+          <t>105.2675763_0.5982484_10550_0020_35</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>105.3749015</v>
+        <v>105.2675763</v>
       </c>
       <c r="C36" t="n">
-        <v>0.4830706</v>
+        <v>0.5982484</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -7830,41 +7705,41 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>cuts/105.3749015,0.4830706_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.2675763,0.5982484_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>cuts/105.3749015,0.4830706_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.2675763,0.5982484_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>cuts/105.3749015,0.4830706_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.2675763,0.5982484_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>cuts/105.3749015,0.4830706_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.2675763,0.5982484_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>cuts/105.3749015,0.4830706_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.2675763,0.5982484_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>105.2675763_0.5982484_10550_0020_36</t>
+          <t>105.2842428_0.6497486_10550_0020_36</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>105.2675763</v>
+        <v>105.2842428</v>
       </c>
       <c r="C37" t="n">
-        <v>0.5982484</v>
+        <v>0.6497486</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -7873,41 +7748,41 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>cuts/105.2675763,0.5982484_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.2842428,0.6497486_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>cuts/105.2675763,0.5982484_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.2842428,0.6497486_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>cuts/105.2675763,0.5982484_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.2842428,0.6497486_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>cuts/105.2675763,0.5982484_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.2842428,0.6497486_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>cuts/105.2675763,0.5982484_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.2842428,0.6497486_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>105.2842428_0.6497486_10550_0020_37</t>
+          <t>105.3760782_0.7864162_10550_0020_37</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>105.2842428</v>
+        <v>105.3760782</v>
       </c>
       <c r="C38" t="n">
-        <v>0.6497486</v>
+        <v>0.7864162</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -7916,41 +7791,41 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>cuts/105.2842428,0.6497486_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.3760782,0.7864162_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>cuts/105.2842428,0.6497486_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.3760782,0.7864162_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>cuts/105.2842428,0.6497486_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.3760782,0.7864162_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>cuts/105.2842428,0.6497486_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.3760782,0.7864162_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>cuts/105.2842428,0.6497486_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.3760782,0.7864162_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>105.3760782_0.7864162_10550_0020_38</t>
+          <t>105.4372473_0.8130832_10550_0020_38</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>105.3760782</v>
+        <v>105.4372473</v>
       </c>
       <c r="C39" t="n">
-        <v>0.7864162</v>
+        <v>0.8130832</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -7959,41 +7834,41 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>cuts/105.3760782,0.7864162_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4372473,0.8130832_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>cuts/105.3760782,0.7864162_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4372473,0.8130832_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>cuts/105.3760782,0.7864162_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4372473,0.8130832_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>cuts/105.3760782,0.7864162_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4372473,0.8130832_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>cuts/105.3760782,0.7864162_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4372473,0.8130832_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>105.4372473_0.8130832_10550_0020_39</t>
+          <t>105.2904077_0.8015820_10550_0020_39</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>105.4372473</v>
+        <v>105.2904077</v>
       </c>
       <c r="C40" t="n">
-        <v>0.8130832</v>
+        <v>0.801582</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -8002,41 +7877,41 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>cuts/105.4372473,0.8130832_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.2904077,0.8015820_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>cuts/105.4372473,0.8130832_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.2904077,0.8015820_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>cuts/105.4372473,0.8130832_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.2904077,0.8015820_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>cuts/105.4372473,0.8130832_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.2904077,0.8015820_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>cuts/105.4372473,0.8130832_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.2904077,0.8015820_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>105.2904077_0.8015820_10550_0020_40</t>
+          <t>105.1085860_-0.0124213_10550_0020_40</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>105.2904077</v>
+        <v>105.108586</v>
       </c>
       <c r="C41" t="n">
-        <v>0.801582</v>
+        <v>-0.0124213</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -8045,41 +7920,41 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>cuts/105.2904077,0.8015820_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.1085860,-0.0124213_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>cuts/105.2904077,0.8015820_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.1085860,-0.0124213_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>cuts/105.2904077,0.8015820_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.1085860,-0.0124213_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>cuts/105.2904077,0.8015820_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.1085860,-0.0124213_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>cuts/105.2904077,0.8015820_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.1085860,-0.0124213_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>105.1085860_-0.0124213_10550_0020_41</t>
+          <t>105.0619031_0.6087441_10550_0020_41</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>105.108586</v>
+        <v>105.0619031</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.0124213</v>
+        <v>0.6087441</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -8088,41 +7963,41 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>cuts/105.1085860,-0.0124213_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.0619031,0.6087441_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>cuts/105.1085860,-0.0124213_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.0619031,0.6087441_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>cuts/105.1085860,-0.0124213_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.0619031,0.6087441_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>cuts/105.1085860,-0.0124213_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.0619031,0.6087441_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>cuts/105.1085860,-0.0124213_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.0619031,0.6087441_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>105.0619031_0.6087441_10550_0020_42</t>
+          <t>105.0612332_0.7272441_10550_0020_42</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>105.0619031</v>
+        <v>105.0612332</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6087441</v>
+        <v>0.7272440999999999</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -8131,41 +8006,41 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>cuts/105.0619031,0.6087441_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.0612332,0.7272441_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>cuts/105.0619031,0.6087441_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.0612332,0.7272441_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>cuts/105.0619031,0.6087441_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.0612332,0.7272441_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>cuts/105.0619031,0.6087441_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.0612332,0.7272441_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>cuts/105.0619031,0.6087441_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.0612332,0.7272441_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>105.0612332_0.7272441_10550_0020_43</t>
+          <t>105.4472489_0.4460832_10550_0020_43</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>105.0612332</v>
+        <v>105.4472489</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7272440999999999</v>
+        <v>0.4460832</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -8174,41 +8049,41 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>cuts/105.0612332,0.7272441_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.4472489,0.4460832_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>cuts/105.0612332,0.7272441_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.4472489,0.4460832_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>cuts/105.0612332,0.7272441_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.4472489,0.4460832_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>cuts/105.0612332,0.7272441_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.4472489,0.4460832_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>cuts/105.0612332,0.7272441_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.4472489,0.4460832_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>105.4472489_0.4460832_10550_0020_44</t>
+          <t>105.7475907_0.5892481_10550_0020_44</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>105.4472489</v>
+        <v>105.7475907</v>
       </c>
       <c r="C45" t="n">
-        <v>0.4460832</v>
+        <v>0.5892481000000001</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -8217,41 +8092,41 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>cuts/105.4472489,0.4460832_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.7475907,0.5892481_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>cuts/105.4472489,0.4460832_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.7475907,0.5892481_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>cuts/105.4472489,0.4460832_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.7475907,0.5892481_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>cuts/105.4472489,0.4460832_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.7475907,0.5892481_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>cuts/105.4472489,0.4460832_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.7475907,0.5892481_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>105.7475907_0.5892481_10550_0020_45</t>
+          <t>105.2143821_0.0171942_10550_0020_45</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>105.7475907</v>
+        <v>105.2143821</v>
       </c>
       <c r="C46" t="n">
-        <v>0.5892481000000001</v>
+        <v>0.0171942</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -8260,41 +8135,41 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>cuts/105.7475907,0.5892481_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.2143821,0.0171942_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>cuts/105.7475907,0.5892481_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.2143821,0.0171942_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>cuts/105.7475907,0.5892481_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.2143821,0.0171942_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>cuts/105.7475907,0.5892481_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.2143821,0.0171942_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>cuts/105.7475907,0.5892481_10550_0020_Azul-3.5micras.jpeg</t>
+          <t>cuts/105.2143821,0.0171942_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>105.2143821_0.0171942_10550_0020_46</t>
+          <t>105.5711048_0.4856490_10550_0020_46</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>105.2143821</v>
+        <v>105.5711048</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0171942</v>
+        <v>0.485649</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -8303,68 +8178,25 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>cuts/105.2143821,0.0171942_10550_0020_RGB-composite.jpeg</t>
+          <t>cuts/105.5711048,0.4856490_10550_0020_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>cuts/105.2143821,0.0171942_10550_0020_Rojo-8micras.jpeg</t>
+          <t>cuts/105.5711048,0.4856490_10550_0020_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>cuts/105.2143821,0.0171942_10550_0020_I3-5.8micras.jpeg</t>
+          <t>cuts/105.5711048,0.4856490_10550_0020_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>cuts/105.2143821,0.0171942_10550_0020_Verde-4.6micras.jpeg</t>
+          <t>cuts/105.5711048,0.4856490_10550_0020_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
-        <is>
-          <t>cuts/105.2143821,0.0171942_10550_0020_Azul-3.5micras.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>105.5711048_0.4856490_10550_0020_47</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>105.5711048</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0.485649</v>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>cuts/105.5711048,0.4856490_10550_0020_RGB-composite.jpeg</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>cuts/105.5711048,0.4856490_10550_0020_Rojo-8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>cuts/105.5711048,0.4856490_10550_0020_I3-5.8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>cuts/105.5711048,0.4856490_10550_0020_Verde-4.6micras.jpeg</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
         <is>
           <t>cuts/105.5711048,0.4856490_10550_0020_Azul-3.5micras.jpeg</t>
         </is>
@@ -8381,7 +8213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R600"/>
+  <dimension ref="A1:R587"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8555,210 +8387,203 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>105.7062490_0.0222487_10550_0020_18</t>
+          <t>105.7364186_0.2367483_10550_0020_18</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>105.7364186_0.2367483_10550_0020_19</t>
+          <t>105.7977563_0.4487473_10550_0020_19</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>105.7977563_0.4487473_10550_0020_20</t>
+          <t>105.6057528_0.5339163_10550_0020_20</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>105.6057528_0.5339163_10550_0020_21</t>
+          <t>105.6185861_0.4862496_10550_0020_21</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>105.6185861_0.4862496_10550_0020_22</t>
+          <t>105.8562640_0.7430795_10550_0020_22</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>105.8562640_0.7430795_10550_0020_23</t>
+          <t>105.4839160_0.8152500_10550_0020_23</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>105.4839160_0.8152500_10550_0020_24</t>
+          <t>105.6207551_0.8000829_10550_0020_24</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>105.6207551_0.8000829_10550_0020_25</t>
+          <t>105.5130838_0.6707500_10550_0020_25</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>105.5130838_0.6707500_10550_0020_26</t>
+          <t>105.5319176_0.5567500_10550_0020_26</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>105.5319176_0.5567500_10550_0020_27</t>
+          <t>105.5240841_0.6047500_10550_0020_27</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>105.5240841_0.6047500_10550_0020_28</t>
+          <t>105.4732496_0.3519166_10550_0020_28</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>105.4732496_0.3519166_10550_0020_29</t>
+          <t>105.4365838_-0.0332501_10550_0020_29</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>105.4365838_-0.0332501_10550_0020_30</t>
+          <t>105.3889170_0.0470830_10550_0020_30</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>105.3889170_0.0470830_10550_0020_31</t>
+          <t>105.4277499_0.1277498_10550_0020_31</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>105.4277499_0.1277498_10550_0020_32</t>
+          <t>105.3647485_0.2809161_10550_0020_32</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>105.3647485_0.2809161_10550_0020_33</t>
+          <t>105.2984131_0.3884154_10550_0020_33</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>105.2984131_0.3884154_10550_0020_34</t>
+          <t>105.3749015_0.4830706_10550_0020_34</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>105.3749015_0.4830706_10550_0020_35</t>
+          <t>105.2675763_0.5982484_10550_0020_35</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>105.2675763_0.5982484_10550_0020_36</t>
+          <t>105.2842428_0.6497486_10550_0020_36</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>105.2842428_0.6497486_10550_0020_37</t>
+          <t>105.3760782_0.7864162_10550_0020_37</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>105.3760782_0.7864162_10550_0020_38</t>
+          <t>105.4372473_0.8130832_10550_0020_38</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>105.4372473_0.8130832_10550_0020_39</t>
+          <t>105.2904077_0.8015820_10550_0020_39</t>
         </is>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>105.2904077_0.8015820_10550_0020_40</t>
+          <t>105.1085860_-0.0124213_10550_0020_40</t>
         </is>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>105.1085860_-0.0124213_10550_0020_41</t>
+          <t>105.0619031_0.6087441_10550_0020_41</t>
         </is>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>105.0619031_0.6087441_10550_0020_42</t>
+          <t>105.0612332_0.7272441_10550_0020_42</t>
         </is>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>105.0612332_0.7272441_10550_0020_43</t>
+          <t>105.4472489_0.4460832_10550_0020_43</t>
         </is>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>105.4472489_0.4460832_10550_0020_44</t>
+          <t>105.7475907_0.5892481_10550_0020_44</t>
         </is>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>105.7475907_0.5892481_10550_0020_45</t>
+          <t>105.2143821_0.0171942_10550_0020_45</t>
         </is>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>105.2143821_0.0171942_10550_0020_46</t>
-        </is>
-      </c>
-    </row>
-    <row r="600">
-      <c r="A600" t="inlineStr">
-        <is>
-          <t>105.5711048_0.4856490_10550_0020_47</t>
+          <t>105.5711048_0.4856490_10550_0020_46</t>
         </is>
       </c>
     </row>

</xml_diff>